<commit_message>
Updates following formal consultation
Updates to documentation based on feedback to formal consultation
</commit_message>
<xml_diff>
--- a/documentation/Heatmap Data Definitions - Latest.xlsx
+++ b/documentation/Heatmap Data Definitions - Latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcmorran/Open Grid Systems Dropbox/Open Grid/Projects/Ofgem/001 LTDS/5-Deliverables/Heatmaps/GitHub/network-heatmaps-api/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5CC1FA-D67D-2943-AF31-B2A89DA70BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3764B80-9BFA-1441-8012-F5C2D2871D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61020" yWindow="2620" windowWidth="33940" windowHeight="20260" activeTab="3" xr2:uid="{D7CEE95D-1517-EC4C-B28A-1A94A9BB30B7}"/>
+    <workbookView xWindow="12980" yWindow="3800" windowWidth="33940" windowHeight="20260" activeTab="8" xr2:uid="{D7CEE95D-1517-EC4C-B28A-1A94A9BB30B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Changes" sheetId="10" r:id="rId1"/>
@@ -298,9 +298,6 @@
     <t>Free text for any additional descriptive data about the constraint</t>
   </si>
   <si>
-    <t>The type of constraint (enumerated field to allow for easier processing/identification)</t>
-  </si>
-  <si>
     <t>FromSubstation</t>
   </si>
   <si>
@@ -430,9 +427,6 @@
     <t>Free text for any additional descriptive data about the curtailment</t>
   </si>
   <si>
-    <t>The type of curtailment (enumerated field to allow for easier processing/identification)</t>
-  </si>
-  <si>
     <t>curtailedBy</t>
   </si>
   <si>
@@ -481,9 +475,6 @@
     <t>The currently contracted generation capacity excluding any that are already contracted or connected  (i.e. do not include any generation that is included in generationConnectedCapacity)</t>
   </si>
   <si>
-    <t>The total firm generation capacity of the substation. Any constraints that impact this capacity should be listed as individual constraints linked to the substation</t>
-  </si>
-  <si>
     <t>Sum of all generation currently connected at the substation. This includes individual generation and storage that are explicitly defined and aggregate value of other connect generation and storage. The value forgenerationConnectedCapacity must be greater than or equal to the sum of the generationConnectedCapacity values in the Generator and Storage elements</t>
   </si>
   <si>
@@ -778,9 +769,6 @@
     <t>The Master Resource ID of the Substation. Where CIM data is being produced for LTDS this ID should be present, persistent across each release of the data and should be the same as the mRID/rdf:ID of the CIM Substation.  If data is produced prior to the CIM LTDS data being published this attribute is optional.</t>
   </si>
   <si>
-    <t xml:space="preserve">The name of the license area. This may be the full text name or an abbreviation that should align with the abbreviations used in the license (e.g. Eastern Power Networks or EPN) </t>
-  </si>
-  <si>
     <t>The human readable name of the substation. This should be consistent with the naming used in LTDS, either Tables 1-8 of existing Excel format, or CIM Substation names for the CIM LTDS data</t>
   </si>
   <si>
@@ -808,9 +796,6 @@
     <t>Changed cardinality to optional</t>
   </si>
   <si>
-    <t>The maximum demand at the substation. This is a normalised value calculated using historic measured values during normal operating conditions .The data represents net demand corrected for any generation at the substation, demand diversity factors, and any other internal processing normally undertaken. All substations at 33kV and above must include demand data; for substations below 33kV, if  corrected, net demand data is not available, the value should be omitted. Users wishing to see separate summer/winter peaks can obtain this from the LTDS data</t>
-  </si>
-  <si>
     <t>The minimum demand at the substation. This is a normalised value calculated using historic measured values during normal operating conditions. The data represents net demand corrected for any generation at the substation, demand diversity factors, and any other internal processing normally undertaken. All substations at 33kV and above must include demand data; for substations below 33kV, if corrected, net demand data is not available, the value should be omitted. Users wishing to see separate summer/winter peaks can obtain this from the LTDS data</t>
   </si>
   <si>
@@ -820,9 +805,6 @@
     <t>The available demand capacity at the substation. This value is calculated based on total firm capacity, maximum demand, connected capacity, quoted capacity, contracted capacity, and any other constraints on the network. The value should reflect the capacity a network operator would make available to a connecting party, which may be calcualted for the most onerous season, or a value based on more detailed analysis and internal policies</t>
   </si>
   <si>
-    <t>Available generation capacity at the substation.This value is calculated based on total firm generation, capacity, demand, connected capacity, quoted capacity, contracted capacity, and any other constraints on the network</t>
-  </si>
-  <si>
     <t>generationAvailabileCapacity</t>
   </si>
   <si>
@@ -844,24 +826,6 @@
     <t>The Master Resource ID of the Circuit.  Where CIM data is being produced for LTDS this ID should be present, persistent across each release of the data and should be the same as the mRID/rdf:ID of the CIM elements.  If data is produced prior to the CIM LTDS data being published this attribute is optional.</t>
   </si>
   <si>
-    <t>The maximum load on the circuit. This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data</t>
-  </si>
-  <si>
-    <t>The minimum demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data.</t>
-  </si>
-  <si>
-    <t>The 99th percentile of demand on the circuit. This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data</t>
-  </si>
-  <si>
-    <t>The 75th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data</t>
-  </si>
-  <si>
-    <t>The 50th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data</t>
-  </si>
-  <si>
-    <t>The 25th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions. All circuits at 33kV and above must include demand data</t>
-  </si>
-  <si>
     <t>Sum of all demand currently connected on the circuit</t>
   </si>
   <si>
@@ -874,9 +838,6 @@
     <t>The Master Resource ID of the demand. Where CIM data is being produced for LTDS this ID should be present, persistent across each release of the data and should be the same as the mRID/rdf:ID of the CIM elements.  If data is produced prior to the CIM LTDS data being published this attribute is optional.</t>
   </si>
   <si>
-    <t>Represents an individual or aggregated demand at the substation. This may represent the aggregation of all generation at a voltage level or individual connected/contracted/quoted generators</t>
-  </si>
-  <si>
     <t>The Master Resource ID of the Generator. Where CIM data is being produced for LTDS this ID should be present, persistent across each release of the data and should be the same as the mRID/rdf:ID of the CIM elements.  If data is produced prior to the CIM LTDS data being published this attribute is optional.</t>
   </si>
   <si>
@@ -938,6 +899,45 @@
   </si>
   <si>
     <t>The Master Resource ID of the Traansformer. Where CIM data is being produced for LTDS this ID should be present, persistent across each release of the data and should be the same as the mRID/rdf:ID of the CIM PowerTransformer.  If data is produced prior to the CIM LTDS data being published this attribute is optional.</t>
+  </si>
+  <si>
+    <t>The name of the license area. This should be the abbreviation used in the license (e.g. EPN for Eastern Power Networks)</t>
+  </si>
+  <si>
+    <t>The maximum demand at the substation. This is a normalised value calculated using historic measured values during normal operating conditions .The data represents net demand without removing the impact of any generation on observed demand at the substation, demand diversity factors, and any other internal processing normally undertaken. All substations at 33kV and above must include demand data; for substations below 33kV, if corrected, net demand data is not available, the value should be omitted. Users wishing to see separate summer/winter peaks can obtain this from the LTDS data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total firm generation capacity of the substation. Any constraints that impact this capacity should be listed as individual constraints linked to the substation. The approach used to calculate this value should be defined in accompanying documentation </t>
+  </si>
+  <si>
+    <t>Available generation capacity at the substation.This value is calculated based on total firm generation, capacity, demand, connected capacity, contracted capacity, and any other constraints on the network</t>
+  </si>
+  <si>
+    <t>The maximum load on the circuit. This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>The minimum demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>The 99th percentile of demand on the circuit. This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>The 75th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>The 50th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>The 25th percentile of demand on the circuit.  This is a value calculated using historic measured values and would not necessarily be corrected for generation on the circuit and normal operating conditions.</t>
+  </si>
+  <si>
+    <t>Represents an individual or aggregated demand at the substation. This may represent the aggregation of all generation at a voltage level or individual connected/contracted/quoted demand</t>
+  </si>
+  <si>
+    <t>The type of constraint (enumerated field to allow for easier processing/identification). Limited to Voltage, Physical or Other.</t>
+  </si>
+  <si>
+    <t>The type of curtailment (enumerated field to allow for easier processing/identification). Limited to Demand or Generation</t>
   </si>
 </sst>
 </file>
@@ -1697,13 +1697,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="D1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1717,7 +1717,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1725,10 +1725,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1739,7 +1739,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1750,7 +1750,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1758,10 +1758,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1769,10 +1769,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1780,10 +1780,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1791,10 +1791,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1802,10 +1802,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1813,10 +1813,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1824,10 +1824,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1835,10 +1835,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1846,10 +1846,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1857,10 +1857,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1868,10 +1868,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -1882,7 +1882,7 @@
         <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
         <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -1904,7 +1904,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -1912,10 +1912,10 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
@@ -1926,7 +1926,7 @@
         <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
@@ -1934,10 +1934,10 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D22" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
@@ -1945,10 +1945,10 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
@@ -1959,7 +1959,7 @@
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
         <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -1986,10 +1986,10 @@
         <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D27" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
@@ -1997,10 +1997,10 @@
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D28" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
@@ -2008,10 +2008,10 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D29" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
@@ -2019,10 +2019,10 @@
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D30" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
@@ -2030,10 +2030,10 @@
         <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -2041,10 +2041,10 @@
         <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -2052,10 +2052,10 @@
         <v>57</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D33" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -2063,10 +2063,10 @@
         <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -2074,10 +2074,10 @@
         <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -2085,40 +2085,40 @@
         <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D37" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -2129,7 +2129,7 @@
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -2140,7 +2140,7 @@
         <v>36</v>
       </c>
       <c r="D41" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -2151,7 +2151,7 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -2173,7 +2173,7 @@
         <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -2184,7 +2184,7 @@
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -2195,7 +2195,7 @@
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -2206,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -2217,7 +2217,7 @@
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -2228,7 +2228,7 @@
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -2236,7 +2236,7 @@
         <v>42</v>
       </c>
       <c r="D50" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2279,15 +2279,15 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C2" s="80"/>
       <c r="D2" s="80"/>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>6</v>
@@ -2312,19 +2312,19 @@
         <v>6</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>155</v>
-      </c>
       <c r="C4" s="27" t="s">
         <v>6</v>
       </c>
@@ -2335,18 +2335,18 @@
         <v>6</v>
       </c>
       <c r="F4" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>170</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>6</v>
@@ -2358,38 +2358,38 @@
         <v>6</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>21</v>
@@ -2404,18 +2404,18 @@
         <v>6</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>6</v>
@@ -2427,18 +2427,18 @@
         <v>6</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>6</v>
@@ -2450,41 +2450,41 @@
         <v>6</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>6</v>
@@ -2496,18 +2496,18 @@
         <v>6</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>6</v>
@@ -2519,18 +2519,18 @@
         <v>6</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>6</v>
@@ -2542,18 +2542,18 @@
         <v>6</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>6</v>
@@ -2565,41 +2565,41 @@
         <v>6</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B15" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>168</v>
-      </c>
       <c r="D15" s="27" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C17" s="55" t="s">
         <v>5</v>
@@ -2611,16 +2611,16 @@
         <v>5</v>
       </c>
       <c r="F17" s="55" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="54" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C18" s="55" t="s">
         <v>57</v>
@@ -2632,7 +2632,7 @@
         <v>57</v>
       </c>
       <c r="F18" s="55" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G18" s="55"/>
     </row>
@@ -2648,8 +2648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE2A9AF-3C70-4340-88A0-CE7B886194C2}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2691,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C2" s="58"/>
       <c r="D2" s="58"/>
@@ -2715,7 +2715,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
@@ -2742,16 +2742,16 @@
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>244</v>
+        <v>285</v>
       </c>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
@@ -2781,7 +2781,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
@@ -2825,7 +2825,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
@@ -2839,7 +2839,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>13</v>
@@ -2914,7 +2914,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
@@ -2936,7 +2936,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
@@ -2958,7 +2958,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
@@ -2968,7 +2968,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>20</v>
@@ -2980,7 +2980,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G15" s="44"/>
       <c r="H15" s="44"/>
@@ -2991,7 +2991,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>20</v>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G16" s="44"/>
       <c r="H16" s="44"/>
@@ -3012,7 +3012,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>20</v>
@@ -3024,7 +3024,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
@@ -3035,7 +3035,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>20</v>
@@ -3047,7 +3047,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G18" s="44"/>
       <c r="H18" s="44"/>
@@ -3058,7 +3058,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>20</v>
@@ -3070,17 +3070,17 @@
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
     </row>
-    <row r="20" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="163" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>20</v>
@@ -3092,7 +3092,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
@@ -3102,7 +3102,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>20</v>
@@ -3114,7 +3114,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
@@ -3124,7 +3124,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>20</v>
@@ -3136,7 +3136,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G22" s="44"/>
       <c r="H22" s="44"/>
@@ -3146,7 +3146,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>20</v>
@@ -3158,7 +3158,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
@@ -3168,7 +3168,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>20</v>
@@ -3180,7 +3180,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="136" x14ac:dyDescent="0.2">
@@ -3188,7 +3188,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>20</v>
@@ -3200,7 +3200,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3208,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>33</v>
@@ -3220,7 +3220,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
@@ -3231,10 +3231,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>12</v>
@@ -3243,18 +3243,18 @@
         <v>6</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
       <c r="I27" s="44"/>
     </row>
-    <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>20</v>
@@ -3266,7 +3266,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>145</v>
+        <v>287</v>
       </c>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
@@ -3276,7 +3276,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>20</v>
@@ -3288,7 +3288,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
@@ -3299,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>20</v>
@@ -3311,7 +3311,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -3322,7 +3322,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>20</v>
@@ -3334,7 +3334,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
@@ -3344,7 +3344,7 @@
         <v>5</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>20</v>
@@ -3356,7 +3356,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
@@ -3366,7 +3366,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>33</v>
@@ -3378,7 +3378,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
@@ -3388,10 +3388,10 @@
         <v>5</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>12</v>
@@ -3400,7 +3400,7 @@
         <v>6</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3411,7 +3411,7 @@
         <v>58</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D35" s="39" t="s">
         <v>16</v>
@@ -3431,7 +3431,7 @@
         <v>60</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D36" s="39" t="s">
         <v>16</v>
@@ -3451,7 +3451,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D37" s="39" t="s">
         <v>16</v>
@@ -3468,10 +3468,10 @@
         <v>5</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D38" s="39" t="s">
         <v>16</v>
@@ -3480,7 +3480,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3491,7 +3491,7 @@
         <v>64</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D39" s="39" t="s">
         <v>16</v>
@@ -3528,7 +3528,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" s="39" t="s">
         <v>20</v>
@@ -3548,7 +3548,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="39" t="s">
         <v>20</v>
@@ -3560,12 +3560,12 @@
         <v>14</v>
       </c>
       <c r="F42" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3573,10 +3573,10 @@
         <v>5</v>
       </c>
       <c r="B44" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="48" t="s">
         <v>115</v>
-      </c>
-      <c r="C44" s="48" t="s">
-        <v>116</v>
       </c>
       <c r="D44" s="48" t="s">
         <v>16</v>
@@ -3585,7 +3585,7 @@
         <v>6</v>
       </c>
       <c r="F44" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3593,19 +3593,19 @@
         <v>5</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3613,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>34</v>
@@ -3625,7 +3625,7 @@
         <v>34</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -3645,7 +3645,7 @@
         <v>69</v>
       </c>
       <c r="F47" s="46" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
@@ -3687,7 +3687,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3695,19 +3695,19 @@
         <v>5</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D50" s="48" t="s">
         <v>45</v>
       </c>
       <c r="E50" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F50" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -3738,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC405D83-9CB1-A44A-97E4-8C22574D93AD}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3774,7 +3774,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -3798,7 +3798,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3818,7 +3818,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3838,7 +3838,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -3846,7 +3846,7 @@
         <v>57</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>20</v>
@@ -3858,15 +3858,15 @@
         <v>14</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>20</v>
@@ -3878,15 +3878,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>20</v>
@@ -3898,15 +3898,15 @@
         <v>14</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>20</v>
@@ -3918,15 +3918,15 @@
         <v>14</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>20</v>
@@ -3938,15 +3938,15 @@
         <v>14</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>20</v>
@@ -3958,7 +3958,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -3966,7 +3966,7 @@
         <v>57</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>33</v>
@@ -3978,7 +3978,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3986,7 +3986,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>20</v>
@@ -3998,7 +3998,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4006,7 +4006,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>20</v>
@@ -4018,7 +4018,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -4026,7 +4026,7 @@
         <v>57</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>20</v>
@@ -4038,7 +4038,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -4046,7 +4046,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>20</v>
@@ -4058,7 +4058,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -4066,7 +4066,7 @@
         <v>57</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>20</v>
@@ -4078,7 +4078,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -4086,7 +4086,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>20</v>
@@ -4098,7 +4098,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4118,7 +4118,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -4126,7 +4126,7 @@
         <v>57</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>7</v>
@@ -4138,7 +4138,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="35" t="s">
         <v>7</v>
@@ -4158,7 +4158,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -4166,19 +4166,19 @@
         <v>57</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -4198,15 +4198,15 @@
         <v>42</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>29</v>
@@ -4230,27 +4230,27 @@
         <v>6</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="33" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -4259,10 +4259,10 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="64"/>
       <c r="D29" s="64"/>
@@ -4271,30 +4271,30 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="D30" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="E30" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="32" t="s">
         <v>97</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="33" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>26</v>
@@ -4318,12 +4318,12 @@
         <v>14</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>24</v>
@@ -4338,7 +4338,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4355,8 +4355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0E145D-850A-5143-B25D-D805EB5B2C13}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4391,10 +4391,10 @@
     </row>
     <row r="2" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="3" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>9</v>
@@ -4418,12 +4418,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>8</v>
@@ -4438,12 +4438,12 @@
         <v>6</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>36</v>
@@ -4458,15 +4458,15 @@
         <v>37</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>20</v>
@@ -4478,15 +4478,15 @@
         <v>14</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>20</v>
@@ -4498,15 +4498,15 @@
         <v>14</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>20</v>
@@ -4518,12 +4518,12 @@
         <v>14</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>38</v>
@@ -4538,12 +4538,12 @@
         <v>14</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>54</v>
@@ -4558,7 +4558,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4635,7 +4635,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4675,7 +4675,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4683,7 +4683,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>20</v>
@@ -4703,7 +4703,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>20</v>
@@ -4715,7 +4715,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4723,7 +4723,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>20</v>
@@ -4735,7 +4735,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4746,7 +4746,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>12</v>
@@ -4853,7 +4853,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4893,7 +4893,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4901,7 +4901,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>20</v>
@@ -4913,7 +4913,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4921,7 +4921,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>20</v>
@@ -4933,7 +4933,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -4941,7 +4941,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>20</v>
@@ -4953,7 +4953,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4961,7 +4961,7 @@
         <v>69</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>20</v>
@@ -4981,7 +4981,7 @@
         <v>69</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>20</v>
@@ -4993,7 +4993,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -5001,7 +5001,7 @@
         <v>69</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>20</v>
@@ -5013,7 +5013,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5024,7 +5024,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>12</v>
@@ -5131,7 +5131,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5162,7 +5162,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>50</v>
@@ -5231,7 +5231,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>20</v>
@@ -5243,7 +5243,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5251,7 +5251,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>20</v>
@@ -5263,7 +5263,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5274,7 +5274,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>12</v>
@@ -5294,7 +5294,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>12</v>
@@ -5320,7 +5320,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5355,7 +5355,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C2" s="78"/>
       <c r="D2" s="78"/>
@@ -5402,7 +5402,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>84</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -5434,8 +5434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D14AE6-78C9-914E-B6BF-D269E096D5BA}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5468,10 +5468,10 @@
     </row>
     <row r="2" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C2" s="78"/>
       <c r="D2" s="78"/>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>8</v>
@@ -5495,12 +5495,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>21</v>
@@ -5515,18 +5515,18 @@
         <v>6</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>12</v>
@@ -5535,15 +5535,15 @@
         <v>6</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>128</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>20</v>
@@ -5555,12 +5555,12 @@
         <v>14</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>54</v>
@@ -5575,18 +5575,18 @@
         <v>14</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>16</v>
@@ -5595,18 +5595,18 @@
         <v>6</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>16</v>
@@ -5615,47 +5615,47 @@
         <v>6</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>